<commit_message>
updated metadata + strategy to handle tick data
</commit_message>
<xml_diff>
--- a/trading_strategy/documentation/P&L results.xlsx
+++ b/trading_strategy/documentation/P&L results.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aparn\Documents\GitHub\cpp_code\trading_strategy\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7CD1F6-DCF6-406A-8F57-F483CD4A3D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F383A5D-9C10-4C99-A194-A38A36A7C254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{55E6D3DF-BA7B-4CA8-AD91-35BEFE8C3FDC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{55E6D3DF-BA7B-4CA8-AD91-35BEFE8C3FDC}"/>
   </bookViews>
   <sheets>
-    <sheet name="P&amp;L results" sheetId="1" r:id="rId1"/>
+    <sheet name="P&amp;L_1s_1" sheetId="1" r:id="rId1"/>
+    <sheet name="P&amp;L 1s_2" sheetId="2" r:id="rId2"/>
+    <sheet name="P&amp;L 1s_3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="16">
   <si>
     <t>Mar</t>
   </si>
@@ -469,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B223F389-5C72-4467-8280-5B3DADD14B66}">
   <dimension ref="B2:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1319,4 +1321,1732 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17569C75-FBC5-434C-98B1-5212EBDC0BFA}">
+  <dimension ref="B2:J32"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
+        <f>F12</f>
+        <v>15171.099999999999</v>
+      </c>
+      <c r="D3" s="2">
+        <f>J12</f>
+        <v>14355.469999999998</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E7" si="0">D3+C3</f>
+        <v>29526.569999999996</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2">
+        <f>F20</f>
+        <v>304</v>
+      </c>
+      <c r="I3" s="2">
+        <f>J20</f>
+        <v>240</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J7" si="1">I3+H3</f>
+        <v>544</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C6" si="2">F13</f>
+        <v>4686.4499999999989</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D6" si="3">J13</f>
+        <v>-1169.1849999999999</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>3517.264999999999</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H6" si="4">F21</f>
+        <v>51</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" ref="I4:I6" si="5">J21</f>
+        <v>32</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="2"/>
+        <v>1735.1</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="3"/>
+        <v>-1420.9389999999999</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>314.16100000000006</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="2"/>
+        <v>4288.2199999999993</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="3"/>
+        <v>1590.11</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>5878.329999999999</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="4"/>
+        <v>53</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="5"/>
+        <v>47</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3">
+        <f>SUM(C3:C6)</f>
+        <v>25880.869999999995</v>
+      </c>
+      <c r="D7" s="3">
+        <f>SUM(D3:D6)</f>
+        <v>13355.455999999998</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>39236.325999999994</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3">
+        <f>SUM(H3:H6)</f>
+        <v>426</v>
+      </c>
+      <c r="I7" s="3">
+        <f>SUM(I3:I6)</f>
+        <v>334</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="1"/>
+        <v>760</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1">
+        <f>C7/1000000*12/COUNT(C3:C6)</f>
+        <v>7.7642609999999987E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <f>D7/1000000*12/COUNT(D3:D6)</f>
+        <v>4.0066367999999991E-2</v>
+      </c>
+      <c r="E8" s="1">
+        <f>E7/1000000*12/COUNT(E3:E6)</f>
+        <v>0.11770897799999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>39744.6</v>
+      </c>
+      <c r="D12" s="2">
+        <v>-44361.1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>19787.599999999999</v>
+      </c>
+      <c r="F12" s="2">
+        <f>SUM(C12:E12)</f>
+        <v>15171.099999999999</v>
+      </c>
+      <c r="G12" s="2">
+        <v>35431.199999999997</v>
+      </c>
+      <c r="H12" s="2">
+        <v>-27197.1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>6121.37</v>
+      </c>
+      <c r="J12" s="2">
+        <f>SUM(G12:I12)</f>
+        <v>14355.469999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>5146.74</v>
+      </c>
+      <c r="D13" s="2">
+        <v>-4479.47</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4019.18</v>
+      </c>
+      <c r="F13" s="2">
+        <f>SUM(C13:E13)</f>
+        <v>4686.4499999999989</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2138.42</v>
+      </c>
+      <c r="H13" s="2">
+        <v>-4015.19</v>
+      </c>
+      <c r="I13" s="2">
+        <v>707.58500000000004</v>
+      </c>
+      <c r="J13" s="2">
+        <f>SUM(G13:I13)</f>
+        <v>-1169.1849999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1768.33</v>
+      </c>
+      <c r="D14" s="2">
+        <v>-1093.8800000000001</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1060.6500000000001</v>
+      </c>
+      <c r="F14" s="2">
+        <f>SUM(C14:E14)</f>
+        <v>1735.1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>-2209.79</v>
+      </c>
+      <c r="I14" s="2">
+        <v>788.851</v>
+      </c>
+      <c r="J14" s="2">
+        <f>SUM(G14:I14)</f>
+        <v>-1420.9389999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4502.28</v>
+      </c>
+      <c r="D15" s="2">
+        <v>-4016.99</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3802.93</v>
+      </c>
+      <c r="F15" s="2">
+        <f>SUM(C15:E15)</f>
+        <v>4288.2199999999993</v>
+      </c>
+      <c r="G15" s="2">
+        <v>3733.45</v>
+      </c>
+      <c r="H15" s="2">
+        <v>-3962.54</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1819.2</v>
+      </c>
+      <c r="J15" s="2">
+        <f>SUM(G15:I15)</f>
+        <v>1590.11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3">
+        <f>SUM(C12:C15)</f>
+        <v>51161.95</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" ref="D16:J16" si="6">SUM(D12:D15)</f>
+        <v>-53951.439999999995</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="6"/>
+        <v>28670.36</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="6"/>
+        <v>25880.869999999995</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="6"/>
+        <v>41303.069999999992</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="6"/>
+        <v>-37384.619999999995</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="6"/>
+        <v>9437.0059999999994</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="6"/>
+        <v>13355.455999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2">
+        <v>58</v>
+      </c>
+      <c r="D20" s="2">
+        <v>131</v>
+      </c>
+      <c r="E20" s="2">
+        <v>115</v>
+      </c>
+      <c r="F20" s="2">
+        <f>SUM(C20:E20)</f>
+        <v>304</v>
+      </c>
+      <c r="G20" s="2">
+        <v>77</v>
+      </c>
+      <c r="H20" s="2">
+        <v>98</v>
+      </c>
+      <c r="I20" s="2">
+        <v>65</v>
+      </c>
+      <c r="J20" s="2">
+        <f>SUM(G20:I20)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2">
+        <v>19</v>
+      </c>
+      <c r="E21" s="2">
+        <v>23</v>
+      </c>
+      <c r="F21" s="2">
+        <f>SUM(C21:E21)</f>
+        <v>51</v>
+      </c>
+      <c r="G21" s="2">
+        <v>7</v>
+      </c>
+      <c r="H21" s="2">
+        <v>14</v>
+      </c>
+      <c r="I21" s="2">
+        <v>11</v>
+      </c>
+      <c r="J21" s="2">
+        <f>SUM(G21:I21)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3</v>
+      </c>
+      <c r="D22" s="2">
+        <v>4</v>
+      </c>
+      <c r="E22" s="2">
+        <v>11</v>
+      </c>
+      <c r="F22" s="2">
+        <f>SUM(C22:E22)</f>
+        <v>18</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <v>8</v>
+      </c>
+      <c r="I22" s="2">
+        <v>7</v>
+      </c>
+      <c r="J22" s="2">
+        <f>SUM(G22:I22)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>4</v>
+      </c>
+      <c r="D23" s="2">
+        <v>20</v>
+      </c>
+      <c r="E23" s="2">
+        <v>29</v>
+      </c>
+      <c r="F23" s="2">
+        <f>SUM(C23:E23)</f>
+        <v>53</v>
+      </c>
+      <c r="G23" s="2">
+        <v>10</v>
+      </c>
+      <c r="H23" s="2">
+        <v>21</v>
+      </c>
+      <c r="I23" s="2">
+        <v>16</v>
+      </c>
+      <c r="J23" s="2">
+        <f>SUM(G23:I23)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3">
+        <f>SUM(C20:C23)</f>
+        <v>74</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" ref="D24:J24" si="7">SUM(D20:D23)</f>
+        <v>174</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="7"/>
+        <v>178</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="7"/>
+        <v>426</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="7"/>
+        <v>94</v>
+      </c>
+      <c r="H24" s="3">
+        <f t="shared" si="7"/>
+        <v>141</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="7"/>
+        <v>99</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="7"/>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="2">
+        <f>IF(C20=0,0,C12/C20)</f>
+        <v>685.25172413793098</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" ref="D28:J28" si="8">IF(D20=0,0,D12/D20)</f>
+        <v>-338.63435114503818</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="8"/>
+        <v>172.06608695652173</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="8"/>
+        <v>49.904934210526314</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="8"/>
+        <v>460.14545454545453</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="8"/>
+        <v>-277.52142857142854</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="8"/>
+        <v>94.174923076923079</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="8"/>
+        <v>59.81445833333332</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" ref="C29:J31" si="9">IF(C21=0,0,C13/C21)</f>
+        <v>571.86</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="9"/>
+        <v>-235.76157894736843</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="9"/>
+        <v>174.74695652173912</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="9"/>
+        <v>91.891176470588221</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="9"/>
+        <v>305.48857142857145</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="9"/>
+        <v>-286.7992857142857</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="9"/>
+        <v>64.325909090909093</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="9"/>
+        <v>-36.537031249999998</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="9"/>
+        <v>589.44333333333327</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="9"/>
+        <v>-273.47000000000003</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="9"/>
+        <v>96.422727272727286</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="9"/>
+        <v>96.394444444444446</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="9"/>
+        <v>-276.22375</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="9"/>
+        <v>112.693</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="9"/>
+        <v>-94.729266666666661</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="9"/>
+        <v>1125.57</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="9"/>
+        <v>-200.84949999999998</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="9"/>
+        <v>131.13551724137932</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="9"/>
+        <v>80.909811320754699</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="9"/>
+        <v>373.34499999999997</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="9"/>
+        <v>-188.69238095238094</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="9"/>
+        <v>113.7</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="9"/>
+        <v>33.832127659574468</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3">
+        <f>C16/C24</f>
+        <v>691.37770270270266</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" ref="D32:J32" si="10">D16/D24</f>
+        <v>-310.06574712643675</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="10"/>
+        <v>161.0694382022472</v>
+      </c>
+      <c r="F32" s="3">
+        <f t="shared" si="10"/>
+        <v>60.753215962441303</v>
+      </c>
+      <c r="G32" s="3">
+        <f t="shared" si="10"/>
+        <v>439.39436170212758</v>
+      </c>
+      <c r="H32" s="3">
+        <f t="shared" si="10"/>
+        <v>-265.13914893617016</v>
+      </c>
+      <c r="I32" s="3">
+        <f t="shared" si="10"/>
+        <v>95.323292929292919</v>
+      </c>
+      <c r="J32" s="3">
+        <f t="shared" si="10"/>
+        <v>39.986395209580834</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:J19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D051D422-6B39-442D-BE35-94914F975353}">
+  <dimension ref="B2:J32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
+        <f>F12</f>
+        <v>15171.099999999999</v>
+      </c>
+      <c r="D3" s="2">
+        <f>J12</f>
+        <v>14355.469999999998</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E7" si="0">D3+C3</f>
+        <v>29526.569999999996</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2">
+        <f>F20</f>
+        <v>304</v>
+      </c>
+      <c r="I3" s="2">
+        <f>J20</f>
+        <v>240</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J7" si="1">I3+H3</f>
+        <v>544</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C6" si="2">F13</f>
+        <v>4686.4499999999989</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D6" si="3">J13</f>
+        <v>-1169.1849999999999</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>3517.264999999999</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H6" si="4">F21</f>
+        <v>51</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" ref="I4:I6" si="5">J21</f>
+        <v>32</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="2"/>
+        <v>1735.1</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="3"/>
+        <v>-1420.9389999999999</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>314.16100000000006</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="2"/>
+        <v>4288.2199999999993</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="3"/>
+        <v>1590.11</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>5878.329999999999</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="4"/>
+        <v>53</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="5"/>
+        <v>47</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3">
+        <f>SUM(C3:C6)</f>
+        <v>25880.869999999995</v>
+      </c>
+      <c r="D7" s="3">
+        <f>SUM(D3:D6)</f>
+        <v>13355.455999999998</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>39236.325999999994</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3">
+        <f>SUM(H3:H6)</f>
+        <v>426</v>
+      </c>
+      <c r="I7" s="3">
+        <f>SUM(I3:I6)</f>
+        <v>334</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="1"/>
+        <v>760</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1">
+        <f>C7/1000000*12/COUNT(C3:C6)</f>
+        <v>7.7642609999999987E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <f>D7/1000000*12/COUNT(D3:D6)</f>
+        <v>4.0066367999999991E-2</v>
+      </c>
+      <c r="E8" s="1">
+        <f>E7/1000000*12/COUNT(E3:E6)</f>
+        <v>0.11770897799999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>39744.6</v>
+      </c>
+      <c r="D12" s="2">
+        <v>-44361.1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>19787.599999999999</v>
+      </c>
+      <c r="F12" s="2">
+        <f>SUM(C12:E12)</f>
+        <v>15171.099999999999</v>
+      </c>
+      <c r="G12" s="2">
+        <v>35431.199999999997</v>
+      </c>
+      <c r="H12" s="2">
+        <v>-27197.1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>6121.37</v>
+      </c>
+      <c r="J12" s="2">
+        <f>SUM(G12:I12)</f>
+        <v>14355.469999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>5146.74</v>
+      </c>
+      <c r="D13" s="2">
+        <v>-4479.47</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4019.18</v>
+      </c>
+      <c r="F13" s="2">
+        <f>SUM(C13:E13)</f>
+        <v>4686.4499999999989</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2138.42</v>
+      </c>
+      <c r="H13" s="2">
+        <v>-4015.19</v>
+      </c>
+      <c r="I13" s="2">
+        <v>707.58500000000004</v>
+      </c>
+      <c r="J13" s="2">
+        <f>SUM(G13:I13)</f>
+        <v>-1169.1849999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1768.33</v>
+      </c>
+      <c r="D14" s="2">
+        <v>-1093.8800000000001</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1060.6500000000001</v>
+      </c>
+      <c r="F14" s="2">
+        <f>SUM(C14:E14)</f>
+        <v>1735.1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>-2209.79</v>
+      </c>
+      <c r="I14" s="2">
+        <v>788.851</v>
+      </c>
+      <c r="J14" s="2">
+        <f>SUM(G14:I14)</f>
+        <v>-1420.9389999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4502.28</v>
+      </c>
+      <c r="D15" s="2">
+        <v>-4016.99</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3802.93</v>
+      </c>
+      <c r="F15" s="2">
+        <f>SUM(C15:E15)</f>
+        <v>4288.2199999999993</v>
+      </c>
+      <c r="G15" s="2">
+        <v>3733.45</v>
+      </c>
+      <c r="H15" s="2">
+        <v>-3962.54</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1819.2</v>
+      </c>
+      <c r="J15" s="2">
+        <f>SUM(G15:I15)</f>
+        <v>1590.11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3">
+        <f>SUM(C12:C15)</f>
+        <v>51161.95</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" ref="D16:J16" si="6">SUM(D12:D15)</f>
+        <v>-53951.439999999995</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="6"/>
+        <v>28670.36</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="6"/>
+        <v>25880.869999999995</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="6"/>
+        <v>41303.069999999992</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="6"/>
+        <v>-37384.619999999995</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="6"/>
+        <v>9437.0059999999994</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="6"/>
+        <v>13355.455999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2">
+        <v>58</v>
+      </c>
+      <c r="D20" s="2">
+        <v>131</v>
+      </c>
+      <c r="E20" s="2">
+        <v>115</v>
+      </c>
+      <c r="F20" s="2">
+        <f>SUM(C20:E20)</f>
+        <v>304</v>
+      </c>
+      <c r="G20" s="2">
+        <v>77</v>
+      </c>
+      <c r="H20" s="2">
+        <v>98</v>
+      </c>
+      <c r="I20" s="2">
+        <v>65</v>
+      </c>
+      <c r="J20" s="2">
+        <f>SUM(G20:I20)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2">
+        <v>19</v>
+      </c>
+      <c r="E21" s="2">
+        <v>23</v>
+      </c>
+      <c r="F21" s="2">
+        <f>SUM(C21:E21)</f>
+        <v>51</v>
+      </c>
+      <c r="G21" s="2">
+        <v>7</v>
+      </c>
+      <c r="H21" s="2">
+        <v>14</v>
+      </c>
+      <c r="I21" s="2">
+        <v>11</v>
+      </c>
+      <c r="J21" s="2">
+        <f>SUM(G21:I21)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3</v>
+      </c>
+      <c r="D22" s="2">
+        <v>4</v>
+      </c>
+      <c r="E22" s="2">
+        <v>11</v>
+      </c>
+      <c r="F22" s="2">
+        <f>SUM(C22:E22)</f>
+        <v>18</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <v>8</v>
+      </c>
+      <c r="I22" s="2">
+        <v>7</v>
+      </c>
+      <c r="J22" s="2">
+        <f>SUM(G22:I22)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>4</v>
+      </c>
+      <c r="D23" s="2">
+        <v>20</v>
+      </c>
+      <c r="E23" s="2">
+        <v>29</v>
+      </c>
+      <c r="F23" s="2">
+        <f>SUM(C23:E23)</f>
+        <v>53</v>
+      </c>
+      <c r="G23" s="2">
+        <v>10</v>
+      </c>
+      <c r="H23" s="2">
+        <v>21</v>
+      </c>
+      <c r="I23" s="2">
+        <v>16</v>
+      </c>
+      <c r="J23" s="2">
+        <f>SUM(G23:I23)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3">
+        <f>SUM(C20:C23)</f>
+        <v>74</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" ref="D24:J24" si="7">SUM(D20:D23)</f>
+        <v>174</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="7"/>
+        <v>178</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="7"/>
+        <v>426</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="7"/>
+        <v>94</v>
+      </c>
+      <c r="H24" s="3">
+        <f t="shared" si="7"/>
+        <v>141</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="7"/>
+        <v>99</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="7"/>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="2">
+        <f>IF(C20=0,0,C12/C20)</f>
+        <v>685.25172413793098</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" ref="D28:J28" si="8">IF(D20=0,0,D12/D20)</f>
+        <v>-338.63435114503818</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="8"/>
+        <v>172.06608695652173</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="8"/>
+        <v>49.904934210526314</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="8"/>
+        <v>460.14545454545453</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="8"/>
+        <v>-277.52142857142854</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="8"/>
+        <v>94.174923076923079</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="8"/>
+        <v>59.81445833333332</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" ref="C29:J31" si="9">IF(C21=0,0,C13/C21)</f>
+        <v>571.86</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="9"/>
+        <v>-235.76157894736843</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="9"/>
+        <v>174.74695652173912</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="9"/>
+        <v>91.891176470588221</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="9"/>
+        <v>305.48857142857145</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="9"/>
+        <v>-286.7992857142857</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="9"/>
+        <v>64.325909090909093</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="9"/>
+        <v>-36.537031249999998</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="9"/>
+        <v>589.44333333333327</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="9"/>
+        <v>-273.47000000000003</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="9"/>
+        <v>96.422727272727286</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="9"/>
+        <v>96.394444444444446</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="9"/>
+        <v>-276.22375</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="9"/>
+        <v>112.693</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="9"/>
+        <v>-94.729266666666661</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="9"/>
+        <v>1125.57</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="9"/>
+        <v>-200.84949999999998</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="9"/>
+        <v>131.13551724137932</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="9"/>
+        <v>80.909811320754699</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="9"/>
+        <v>373.34499999999997</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="9"/>
+        <v>-188.69238095238094</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="9"/>
+        <v>113.7</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="9"/>
+        <v>33.832127659574468</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3">
+        <f>C16/C24</f>
+        <v>691.37770270270266</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" ref="D32:J32" si="10">D16/D24</f>
+        <v>-310.06574712643675</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="10"/>
+        <v>161.0694382022472</v>
+      </c>
+      <c r="F32" s="3">
+        <f t="shared" si="10"/>
+        <v>60.753215962441303</v>
+      </c>
+      <c r="G32" s="3">
+        <f t="shared" si="10"/>
+        <v>439.39436170212758</v>
+      </c>
+      <c r="H32" s="3">
+        <f t="shared" si="10"/>
+        <v>-265.13914893617016</v>
+      </c>
+      <c r="I32" s="3">
+        <f t="shared" si="10"/>
+        <v>95.323292929292919</v>
+      </c>
+      <c r="J32" s="3">
+        <f t="shared" si="10"/>
+        <v>39.986395209580834</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:J19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
move calibrated params into ccyPairDef struct + bug fixes
</commit_message>
<xml_diff>
--- a/trading_strategy/documentation/P&L results.xlsx
+++ b/trading_strategy/documentation/P&L results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aparn\Documents\GitHub\cpp_code\trading_strategy\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD4EDCD-C5A6-4C7D-BD38-3A9DED245FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5344DCE3-9042-4350-83A1-FDD13C0DD8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{55E6D3DF-BA7B-4CA8-AD91-35BEFE8C3FDC}"/>
   </bookViews>
@@ -155,10 +155,10 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="38" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="38" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -498,7 +498,7 @@
   <dimension ref="B2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,10 +507,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="str">
@@ -554,15 +554,15 @@
       </c>
       <c r="C4" s="2">
         <f>'P&amp;L 1s'!C3</f>
-        <v>3557.5600000000013</v>
+        <v>1372.8100000000013</v>
       </c>
       <c r="D4" s="2">
         <f>'P&amp;L 1s'!D3</f>
-        <v>4440.2599999999984</v>
+        <v>5371.6100000000006</v>
       </c>
       <c r="E4" s="2">
         <f>'P&amp;L 1s'!E3</f>
-        <v>7997.82</v>
+        <v>6744.4200000000019</v>
       </c>
       <c r="G4" t="str">
         <f>'P&amp;L 1s'!G3</f>
@@ -570,15 +570,15 @@
       </c>
       <c r="H4" s="2">
         <f>'P&amp;L 1s'!H3</f>
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I4" s="2">
         <f>'P&amp;L 1s'!I3</f>
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="J4" s="2">
         <f>'P&amp;L 1s'!J3</f>
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="K4" s="2"/>
     </row>
@@ -589,15 +589,15 @@
       </c>
       <c r="C5" s="2">
         <f>'P&amp;L 1s'!C4</f>
-        <v>13973.900000000001</v>
+        <v>12620.699999999997</v>
       </c>
       <c r="D5" s="2">
         <f>'P&amp;L 1s'!D4</f>
-        <v>544.08000000000129</v>
+        <v>2592.1399999999985</v>
       </c>
       <c r="E5" s="2">
         <f>'P&amp;L 1s'!E4</f>
-        <v>14517.980000000003</v>
+        <v>15212.839999999997</v>
       </c>
       <c r="G5" t="str">
         <f>'P&amp;L 1s'!G4</f>
@@ -605,15 +605,15 @@
       </c>
       <c r="H5" s="2">
         <f>'P&amp;L 1s'!H4</f>
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="I5" s="2">
         <f>'P&amp;L 1s'!I4</f>
-        <v>215</v>
+        <v>188</v>
       </c>
       <c r="J5" s="2">
         <f>'P&amp;L 1s'!J4</f>
-        <v>481</v>
+        <v>442</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -624,7 +624,7 @@
       </c>
       <c r="C6" s="2">
         <f>'P&amp;L 1s'!C5</f>
-        <v>5064.75</v>
+        <v>4126.82</v>
       </c>
       <c r="D6" s="2">
         <f>'P&amp;L 1s'!D5</f>
@@ -632,7 +632,7 @@
       </c>
       <c r="E6" s="2">
         <f>'P&amp;L 1s'!E5</f>
-        <v>4621.2241999999997</v>
+        <v>3683.2941999999998</v>
       </c>
       <c r="G6" t="str">
         <f>'P&amp;L 1s'!G5</f>
@@ -640,7 +640,7 @@
       </c>
       <c r="H6" s="2">
         <f>'P&amp;L 1s'!H5</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I6" s="2">
         <f>'P&amp;L 1s'!I5</f>
@@ -648,7 +648,7 @@
       </c>
       <c r="J6" s="2">
         <f>'P&amp;L 1s'!J5</f>
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K6" s="2"/>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="C7" s="2">
         <f>'P&amp;L 1s'!C6</f>
-        <v>1841.62</v>
+        <v>1768.6999999999998</v>
       </c>
       <c r="D7" s="2">
         <f>'P&amp;L 1s'!D6</f>
@@ -667,7 +667,7 @@
       </c>
       <c r="E7" s="2">
         <f>'P&amp;L 1s'!E6</f>
-        <v>-34.193900000000212</v>
+        <v>-107.11390000000029</v>
       </c>
       <c r="G7" t="str">
         <f>'P&amp;L 1s'!G6</f>
@@ -694,15 +694,15 @@
       </c>
       <c r="C8" s="2">
         <f>'P&amp;L 1s'!C7</f>
-        <v>2747.9899999999993</v>
+        <v>2661.27</v>
       </c>
       <c r="D8" s="2">
         <f>'P&amp;L 1s'!D7</f>
-        <v>621.24099999999976</v>
+        <v>52.490999999999985</v>
       </c>
       <c r="E8" s="2">
         <f>'P&amp;L 1s'!E7</f>
-        <v>3369.2309999999989</v>
+        <v>2713.761</v>
       </c>
       <c r="G8" t="str">
         <f>'P&amp;L 1s'!G7</f>
@@ -710,15 +710,15 @@
       </c>
       <c r="H8" s="2">
         <f>'P&amp;L 1s'!H7</f>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I8" s="2">
         <f>'P&amp;L 1s'!I7</f>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J8" s="2">
         <f>'P&amp;L 1s'!J7</f>
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K8" s="2"/>
     </row>
@@ -726,28 +726,28 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3">
         <f>'P&amp;L 1s'!C8</f>
-        <v>27185.82</v>
+        <v>22550.3</v>
       </c>
       <c r="D9" s="3">
         <f>'P&amp;L 1s'!D8</f>
-        <v>3286.2412999999997</v>
+        <v>5696.9012999999986</v>
       </c>
       <c r="E9" s="3">
         <f>'P&amp;L 1s'!E8</f>
-        <v>30472.061300000001</v>
+        <v>28247.201299999997</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3">
         <f>'P&amp;L 1s'!H8</f>
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="I9" s="3">
         <f>'P&amp;L 1s'!I8</f>
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="J9" s="3">
         <f>'P&amp;L 1s'!J8</f>
-        <v>662</v>
+        <v>619</v>
       </c>
       <c r="K9" s="2"/>
     </row>
@@ -758,15 +758,15 @@
       </c>
       <c r="C10" s="1">
         <f>'P&amp;L 1s'!C9</f>
-        <v>6.5245968000000001E-2</v>
+        <v>5.4120719999999997E-2</v>
       </c>
       <c r="D10" s="1">
         <f>'P&amp;L 1s'!D9</f>
-        <v>7.8869791200000001E-3</v>
+        <v>1.3672563119999998E-2</v>
       </c>
       <c r="E10" s="1">
         <f>'P&amp;L 1s'!E9</f>
-        <v>7.313294712E-2</v>
+        <v>6.7793283119999992E-2</v>
       </c>
       <c r="K10" s="2"/>
     </row>
@@ -783,10 +783,10 @@
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="4"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="str">
@@ -829,15 +829,15 @@
       </c>
       <c r="C14" s="2">
         <f>'P&amp;L tick'!C3</f>
-        <v>4893.4400000000014</v>
+        <v>2735.95</v>
       </c>
       <c r="D14" s="2">
         <f>'P&amp;L tick'!D3</f>
-        <v>6285.0399999999991</v>
+        <v>5194.420000000001</v>
       </c>
       <c r="E14" s="2">
         <f>'P&amp;L tick'!E3</f>
-        <v>11178.48</v>
+        <v>7930.3700000000008</v>
       </c>
       <c r="G14" t="str">
         <f>'P&amp;L tick'!G3</f>
@@ -845,15 +845,15 @@
       </c>
       <c r="H14" s="2">
         <f>'P&amp;L tick'!H3</f>
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I14" s="2">
         <f>'P&amp;L tick'!I3</f>
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="J14" s="2">
         <f>'P&amp;L tick'!J3</f>
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
@@ -863,15 +863,15 @@
       </c>
       <c r="C15" s="2">
         <f>'P&amp;L tick'!C4</f>
-        <v>8588.7999999999956</v>
+        <v>8735.7999999999993</v>
       </c>
       <c r="D15" s="2">
         <f>'P&amp;L tick'!D4</f>
-        <v>16291.459999999995</v>
+        <v>15285.559999999998</v>
       </c>
       <c r="E15" s="2">
         <f>'P&amp;L tick'!E4</f>
-        <v>24880.259999999991</v>
+        <v>24021.359999999997</v>
       </c>
       <c r="G15" t="str">
         <f>'P&amp;L tick'!G4</f>
@@ -879,15 +879,15 @@
       </c>
       <c r="H15" s="2">
         <f>'P&amp;L tick'!H4</f>
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="I15" s="2">
         <f>'P&amp;L tick'!I4</f>
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="J15" s="2">
         <f>'P&amp;L tick'!J4</f>
-        <v>562</v>
+        <v>538</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
@@ -897,7 +897,7 @@
       </c>
       <c r="C16" s="2">
         <f>'P&amp;L tick'!C5</f>
-        <v>804.14000000000033</v>
+        <v>992.12999999999988</v>
       </c>
       <c r="D16" s="2">
         <f>'P&amp;L tick'!D5</f>
@@ -905,7 +905,7 @@
       </c>
       <c r="E16" s="2">
         <f>'P&amp;L tick'!E5</f>
-        <v>-1129.8050000000003</v>
+        <v>-941.81500000000074</v>
       </c>
       <c r="G16" t="str">
         <f>'P&amp;L tick'!G5</f>
@@ -931,7 +931,7 @@
       </c>
       <c r="C17" s="2">
         <f>'P&amp;L tick'!C6</f>
-        <v>913.93000000000006</v>
+        <v>659.05300000000011</v>
       </c>
       <c r="D17" s="2">
         <f>'P&amp;L tick'!D6</f>
@@ -939,7 +939,7 @@
       </c>
       <c r="E17" s="2">
         <f>'P&amp;L tick'!E6</f>
-        <v>1146.5230000000001</v>
+        <v>891.64600000000019</v>
       </c>
       <c r="G17" t="str">
         <f>'P&amp;L tick'!G6</f>
@@ -965,7 +965,7 @@
       </c>
       <c r="C18" s="2">
         <f>'P&amp;L tick'!C7</f>
-        <v>1805.46</v>
+        <v>1980.9599999999996</v>
       </c>
       <c r="D18" s="2">
         <f>'P&amp;L tick'!D7</f>
@@ -973,7 +973,7 @@
       </c>
       <c r="E18" s="2">
         <f>'P&amp;L tick'!E7</f>
-        <v>-930.81999999999971</v>
+        <v>-755.32000000000016</v>
       </c>
       <c r="G18" t="str">
         <f>'P&amp;L tick'!G7</f>
@@ -981,7 +981,7 @@
       </c>
       <c r="H18" s="2">
         <f>'P&amp;L tick'!H7</f>
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I18" s="2">
         <f>'P&amp;L tick'!I7</f>
@@ -989,35 +989,35 @@
       </c>
       <c r="J18" s="2">
         <f>'P&amp;L tick'!J7</f>
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="3">
         <f>'P&amp;L tick'!C8</f>
-        <v>17005.769999999997</v>
+        <v>15103.892999999998</v>
       </c>
       <c r="D19" s="3">
         <f>'P&amp;L tick'!D8</f>
-        <v>18138.867999999995</v>
+        <v>16042.348000000002</v>
       </c>
       <c r="E19" s="3">
         <f>'P&amp;L tick'!E8</f>
-        <v>35144.637999999992</v>
+        <v>31146.241000000002</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3">
         <f>'P&amp;L tick'!H8</f>
-        <v>480</v>
+        <v>469</v>
       </c>
       <c r="I19" s="3">
         <f>'P&amp;L tick'!I8</f>
-        <v>472</v>
+        <v>457</v>
       </c>
       <c r="J19" s="3">
         <f>'P&amp;L tick'!J8</f>
-        <v>952</v>
+        <v>926</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
@@ -1027,15 +1027,15 @@
       </c>
       <c r="C20" s="1">
         <f>'P&amp;L tick'!C9</f>
-        <v>4.0813847999999993E-2</v>
+        <v>3.6249343199999992E-2</v>
       </c>
       <c r="D20" s="1">
         <f>'P&amp;L tick'!D9</f>
-        <v>4.3533283199999988E-2</v>
+        <v>3.8501635200000009E-2</v>
       </c>
       <c r="E20" s="1">
         <f>'P&amp;L tick'!E9</f>
-        <v>8.4347131199999981E-2</v>
+        <v>7.4750978400000001E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1052,7 +1052,7 @@
   <dimension ref="B2:J36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1095,30 +1095,30 @@
       </c>
       <c r="C3" s="2">
         <f>F13</f>
-        <v>3557.5600000000013</v>
+        <v>1372.8100000000013</v>
       </c>
       <c r="D3" s="2">
         <f>J13</f>
-        <v>4440.2599999999984</v>
+        <v>5371.6100000000006</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3" si="0">D3+C3</f>
-        <v>7997.82</v>
+        <v>6744.4200000000019</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
       </c>
       <c r="H3" s="2">
         <f>F22</f>
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I3" s="2">
         <f>J22</f>
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ref="J3" si="1">I3+H3</f>
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
@@ -1127,30 +1127,30 @@
       </c>
       <c r="C4" s="2">
         <f>F14</f>
-        <v>13973.900000000001</v>
+        <v>12620.699999999997</v>
       </c>
       <c r="D4" s="2">
         <f>J14</f>
-        <v>544.08000000000129</v>
+        <v>2592.1399999999985</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" ref="E4:E8" si="2">D4+C4</f>
-        <v>14517.980000000003</v>
+        <v>15212.839999999997</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="2">
         <f>F23</f>
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="I4" s="2">
         <f>J23</f>
-        <v>215</v>
+        <v>188</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" ref="J4:J8" si="3">I4+H4</f>
-        <v>481</v>
+        <v>442</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ref="C5:C7" si="4">F15</f>
-        <v>5064.75</v>
+        <v>4126.82</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" ref="D5:D7" si="5">J15</f>
@@ -1167,14 +1167,14 @@
       </c>
       <c r="E5" s="2">
         <f t="shared" si="2"/>
-        <v>4621.2241999999997</v>
+        <v>3683.2941999999998</v>
       </c>
       <c r="G5" t="s">
         <v>0</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" ref="H5:H7" si="6">F24</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" ref="I5:I7" si="7">J24</f>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="J5" s="2">
         <f t="shared" si="3"/>
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" si="4"/>
-        <v>1841.62</v>
+        <v>1768.6999999999998</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="5"/>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="E6" s="2">
         <f t="shared" si="2"/>
-        <v>-34.193900000000212</v>
+        <v>-107.11390000000029</v>
       </c>
       <c r="G6" t="s">
         <v>1</v>
@@ -1223,58 +1223,58 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" si="4"/>
-        <v>2747.9899999999993</v>
+        <v>2661.27</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="5"/>
-        <v>621.24099999999976</v>
+        <v>52.490999999999985</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="2"/>
-        <v>3369.2309999999989</v>
+        <v>2713.761</v>
       </c>
       <c r="G7" t="s">
         <v>2</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="6"/>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="7"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="3"/>
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
       <c r="C8" s="3">
         <f>SUM(C3:C7)</f>
-        <v>27185.82</v>
+        <v>22550.3</v>
       </c>
       <c r="D8" s="3">
         <f>SUM(D3:D7)</f>
-        <v>3286.2412999999997</v>
+        <v>5696.9012999999986</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="2"/>
-        <v>30472.061300000001</v>
+        <v>28247.201299999997</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3">
         <f>SUM(H4:H7)</f>
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="I8" s="3">
         <f>SUM(I4:I7)</f>
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" si="3"/>
-        <v>662</v>
+        <v>619</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
@@ -1283,32 +1283,32 @@
       </c>
       <c r="C9" s="1">
         <f>C8/1000000*12/COUNT(C3:C7)</f>
-        <v>6.5245968000000001E-2</v>
+        <v>5.4120719999999997E-2</v>
       </c>
       <c r="D9" s="1">
         <f>D8/1000000*12/COUNT(D3:D7)</f>
-        <v>7.8869791200000001E-3</v>
+        <v>1.3672563119999998E-2</v>
       </c>
       <c r="E9" s="1">
         <f>E8/1000000*12/COUNT(E3:E7)</f>
-        <v>7.313294712E-2</v>
+        <v>6.7793283119999992E-2</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4" t="s">
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1325,7 +1325,7 @@
       <c r="E12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="3" t="s">
         <v>10</v>
       </c>
@@ -1335,37 +1335,37 @@
       <c r="I12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="4"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="2">
-        <v>12940.9</v>
+        <v>13048.9</v>
       </c>
       <c r="D13" s="2">
-        <v>-18466.599999999999</v>
+        <v>-18610.599999999999</v>
       </c>
       <c r="E13" s="2">
-        <v>9083.26</v>
+        <v>6934.51</v>
       </c>
       <c r="F13" s="2">
         <f>SUM(C13:E13)</f>
-        <v>3557.5600000000013</v>
+        <v>1372.8100000000013</v>
       </c>
       <c r="G13" s="2">
-        <v>13086.8</v>
+        <v>12670.1</v>
       </c>
       <c r="H13" s="2">
-        <v>-9856.2800000000007</v>
+        <v>-8395.59</v>
       </c>
       <c r="I13" s="2">
-        <v>1209.74</v>
+        <v>1097.0999999999999</v>
       </c>
       <c r="J13" s="2">
         <f>SUM(G13:I13)</f>
-        <v>4440.2599999999984</v>
+        <v>5371.6100000000006</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
@@ -1373,30 +1373,30 @@
         <v>3</v>
       </c>
       <c r="C14" s="2">
-        <v>32331.599999999999</v>
+        <v>30792.2</v>
       </c>
       <c r="D14" s="2">
-        <v>-34970.199999999997</v>
+        <v>-34454.800000000003</v>
       </c>
       <c r="E14" s="2">
-        <v>16612.5</v>
+        <v>16283.3</v>
       </c>
       <c r="F14" s="2">
         <f>SUM(C14:E14)</f>
-        <v>13973.900000000001</v>
+        <v>12620.699999999997</v>
       </c>
       <c r="G14" s="2">
-        <v>26740.9</v>
+        <v>23226.5</v>
       </c>
       <c r="H14" s="2">
-        <v>-28264.5</v>
+        <v>-23942.9</v>
       </c>
       <c r="I14" s="2">
-        <v>2067.6799999999998</v>
+        <v>3308.54</v>
       </c>
       <c r="J14" s="2">
         <f>SUM(G14:I14)</f>
-        <v>544.08000000000129</v>
+        <v>2592.1399999999985</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
@@ -1407,14 +1407,14 @@
         <v>3414.79</v>
       </c>
       <c r="D15" s="2">
-        <v>-3131.63</v>
+        <v>-3666.65</v>
       </c>
       <c r="E15" s="2">
-        <v>4781.59</v>
+        <v>4378.68</v>
       </c>
       <c r="F15" s="2">
         <f>SUM(C15:E15)</f>
-        <v>5064.75</v>
+        <v>4126.82</v>
       </c>
       <c r="G15" s="2">
         <v>2177.77</v>
@@ -1441,11 +1441,11 @@
         <v>-1093.8800000000001</v>
       </c>
       <c r="E16" s="2">
-        <v>1507.38</v>
+        <v>1434.46</v>
       </c>
       <c r="F16" s="2">
         <f>SUM(C16:E16)</f>
-        <v>1841.62</v>
+        <v>1768.6999999999998</v>
       </c>
       <c r="G16" s="2">
         <v>0</v>
@@ -1469,17 +1469,17 @@
         <v>4502.28</v>
       </c>
       <c r="D17" s="2">
-        <v>-4222.93</v>
+        <v>-3998.35</v>
       </c>
       <c r="E17" s="2">
-        <v>2468.64</v>
+        <v>2157.34</v>
       </c>
       <c r="F17" s="2">
         <f>SUM(C17:E17)</f>
-        <v>2747.9899999999993</v>
+        <v>2661.27</v>
       </c>
       <c r="G17" s="2">
-        <v>2511.1799999999998</v>
+        <v>1942.43</v>
       </c>
       <c r="H17" s="2">
         <v>-2709.88</v>
@@ -1489,59 +1489,59 @@
       </c>
       <c r="J17" s="2">
         <f>SUM(G17:I17)</f>
-        <v>621.24099999999976</v>
+        <v>52.490999999999985</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="C18" s="3">
         <f>SUM(C13:C17)</f>
-        <v>54617.69</v>
+        <v>53186.29</v>
       </c>
       <c r="D18" s="3">
         <f t="shared" ref="D18:J18" si="8">SUM(D13:D17)</f>
-        <v>-61885.239999999991</v>
+        <v>-61824.28</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" si="8"/>
-        <v>34453.370000000003</v>
+        <v>31188.289999999997</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="8"/>
-        <v>27185.82</v>
+        <v>22550.3</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="8"/>
-        <v>44516.649999999994</v>
+        <v>40016.799999999996</v>
       </c>
       <c r="H18" s="3">
         <f t="shared" si="8"/>
-        <v>-45293.5</v>
+        <v>-39511.21</v>
       </c>
       <c r="I18" s="3">
         <f t="shared" si="8"/>
-        <v>4063.0913</v>
+        <v>5191.3112999999994</v>
       </c>
       <c r="J18" s="3">
         <f t="shared" si="8"/>
-        <v>3286.2412999999997</v>
+        <v>5696.9012999999986</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4" t="s">
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1558,7 +1558,7 @@
       <c r="E21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="3" t="s">
         <v>10</v>
       </c>
@@ -1568,7 +1568,7 @@
       <c r="I21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J21" s="4"/>
+      <c r="J21" s="5"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
@@ -1578,27 +1578,27 @@
         <v>21</v>
       </c>
       <c r="D22" s="2">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E22" s="2">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F22" s="2">
         <f>SUM(C22:E22)</f>
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="G22" s="2">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H22" s="2">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I22" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J22" s="2">
         <f>SUM(G22:I22)</f>
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
@@ -1606,30 +1606,30 @@
         <v>3</v>
       </c>
       <c r="C23" s="2">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D23" s="2">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E23" s="2">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F23" s="2">
         <f>SUM(C23:E23)</f>
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="G23" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="H23" s="2">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="I23" s="2">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="J23" s="2">
         <f>SUM(G23:I23)</f>
-        <v>215</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
@@ -1640,14 +1640,14 @@
         <v>7</v>
       </c>
       <c r="D24" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E24" s="2">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F24" s="2">
         <f>SUM(C24:E24)</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G24" s="2">
         <v>6</v>
@@ -1702,17 +1702,17 @@
         <v>4</v>
       </c>
       <c r="D26" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E26" s="2">
         <v>24</v>
       </c>
       <c r="F26" s="2">
         <f>SUM(C26:E26)</f>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G26" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H26" s="2">
         <v>16</v>
@@ -1722,59 +1722,59 @@
       </c>
       <c r="J26" s="2">
         <f>SUM(G26:I26)</f>
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="3"/>
       <c r="C27" s="3">
         <f>SUM(C22:C26)</f>
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" ref="D27:J27" si="9">SUM(D22:D26)</f>
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="9"/>
-        <v>519</v>
+        <v>499</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="9"/>
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="H27" s="3">
         <f t="shared" si="9"/>
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="I27" s="3">
         <f t="shared" si="9"/>
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J27" s="3">
         <f t="shared" si="9"/>
-        <v>359</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4" t="s">
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4" t="s">
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1791,7 +1791,7 @@
       <c r="E30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="4"/>
+      <c r="F30" s="5"/>
       <c r="G30" s="3" t="s">
         <v>10</v>
       </c>
@@ -1801,43 +1801,43 @@
       <c r="I30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J30" s="4"/>
+      <c r="J30" s="5"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="2">
-        <f>IF(C22=0,0,C13/C22)</f>
-        <v>616.23333333333335</v>
+        <f t="shared" ref="C31:J35" si="10">IF(C22=0,0,C13/C22)</f>
+        <v>621.37619047619046</v>
       </c>
       <c r="D31" s="2">
-        <f>IF(D22=0,0,D13/D22)</f>
-        <v>-297.84838709677416</v>
+        <f t="shared" si="10"/>
+        <v>-305.09180327868847</v>
       </c>
       <c r="E31" s="2">
-        <f>IF(E22=0,0,E13/E22)</f>
-        <v>148.90590163934428</v>
+        <f t="shared" si="10"/>
+        <v>123.83053571428572</v>
       </c>
       <c r="F31" s="2">
-        <f>IF(F22=0,0,F13/F22)</f>
-        <v>24.705277777777788</v>
+        <f t="shared" si="10"/>
+        <v>9.9478985507246467</v>
       </c>
       <c r="G31" s="2">
-        <f>IF(G22=0,0,G13/G22)</f>
-        <v>727.04444444444437</v>
+        <f t="shared" si="10"/>
+        <v>844.6733333333334</v>
       </c>
       <c r="H31" s="2">
-        <f>IF(H22=0,0,H13/H22)</f>
-        <v>-266.38594594594599</v>
+        <f t="shared" si="10"/>
+        <v>-246.92911764705883</v>
       </c>
       <c r="I31" s="2">
-        <f>IF(I22=0,0,I13/I22)</f>
-        <v>71.161176470588231</v>
+        <f t="shared" si="10"/>
+        <v>68.568749999999994</v>
       </c>
       <c r="J31" s="2">
-        <f>IF(J22=0,0,J13/J22)</f>
-        <v>61.670277777777756</v>
+        <f t="shared" si="10"/>
+        <v>82.640153846153851</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
@@ -1845,36 +1845,36 @@
         <v>3</v>
       </c>
       <c r="C32" s="2">
-        <f>IF(C23=0,0,C14/C23)</f>
-        <v>598.73333333333335</v>
+        <f t="shared" si="10"/>
+        <v>628.41224489795923</v>
       </c>
       <c r="D32" s="2">
-        <f>IF(D23=0,0,D14/D23)</f>
-        <v>-317.91090909090906</v>
+        <f t="shared" si="10"/>
+        <v>-319.02592592592595</v>
       </c>
       <c r="E32" s="2">
-        <f>IF(E23=0,0,E14/E23)</f>
-        <v>162.86764705882354</v>
+        <f t="shared" si="10"/>
+        <v>167.86907216494845</v>
       </c>
       <c r="F32" s="2">
-        <f>IF(F23=0,0,F14/F23)</f>
-        <v>52.533458646616545</v>
+        <f t="shared" si="10"/>
+        <v>49.687795275590538</v>
       </c>
       <c r="G32" s="2">
-        <f>IF(G23=0,0,G14/G23)</f>
-        <v>504.54528301886796</v>
+        <f t="shared" si="10"/>
+        <v>540.15116279069764</v>
       </c>
       <c r="H32" s="2">
-        <f>IF(H23=0,0,H14/H23)</f>
-        <v>-277.10294117647061</v>
+        <f t="shared" si="10"/>
+        <v>-257.45053763440859</v>
       </c>
       <c r="I32" s="2">
-        <f>IF(I23=0,0,I14/I23)</f>
-        <v>34.461333333333329</v>
+        <f t="shared" si="10"/>
+        <v>63.62576923076923</v>
       </c>
       <c r="J32" s="2">
-        <f>IF(J23=0,0,J14/J23)</f>
-        <v>2.5306046511627969</v>
+        <f t="shared" si="10"/>
+        <v>13.787978723404247</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
@@ -1882,35 +1882,35 @@
         <v>0</v>
       </c>
       <c r="C33" s="2">
-        <f>IF(C24=0,0,C15/C24)</f>
+        <f t="shared" si="10"/>
         <v>487.82714285714286</v>
       </c>
       <c r="D33" s="2">
-        <f>IF(D24=0,0,D15/D24)</f>
-        <v>-195.72687500000001</v>
+        <f t="shared" si="10"/>
+        <v>-215.68529411764706</v>
       </c>
       <c r="E33" s="2">
-        <f>IF(E24=0,0,E15/E24)</f>
-        <v>227.69476190476192</v>
+        <f t="shared" si="10"/>
+        <v>230.45684210526318</v>
       </c>
       <c r="F33" s="2">
-        <f>IF(F24=0,0,F15/F24)</f>
-        <v>115.10795454545455</v>
+        <f t="shared" si="10"/>
+        <v>95.972558139534883</v>
       </c>
       <c r="G33" s="2">
-        <f>IF(G24=0,0,G15/G24)</f>
+        <f t="shared" si="10"/>
         <v>362.96166666666664</v>
       </c>
       <c r="H33" s="2">
-        <f>IF(H24=0,0,H15/H24)</f>
+        <f t="shared" si="10"/>
         <v>-216.64083333333335</v>
       </c>
       <c r="I33" s="2">
-        <f>IF(I24=0,0,I15/I24)</f>
+        <f t="shared" si="10"/>
         <v>-1.9641636363636363</v>
       </c>
       <c r="J33" s="2">
-        <f>IF(J24=0,0,J15/J24)</f>
+        <f t="shared" si="10"/>
         <v>-15.293993103448278</v>
       </c>
     </row>
@@ -1919,35 +1919,35 @@
         <v>1</v>
       </c>
       <c r="C34" s="2">
-        <f>IF(C25=0,0,C16/C25)</f>
+        <f t="shared" si="10"/>
         <v>714.06</v>
       </c>
       <c r="D34" s="2">
-        <f>IF(D25=0,0,D16/D25)</f>
+        <f t="shared" si="10"/>
         <v>-273.47000000000003</v>
       </c>
       <c r="E34" s="2">
-        <f>IF(E25=0,0,E16/E25)</f>
-        <v>137.03454545454545</v>
+        <f t="shared" si="10"/>
+        <v>130.40545454545455</v>
       </c>
       <c r="F34" s="2">
-        <f>IF(F25=0,0,F16/F25)</f>
-        <v>108.33058823529412</v>
+        <f t="shared" si="10"/>
+        <v>104.04117647058823</v>
       </c>
       <c r="G34" s="2">
-        <f>IF(G25=0,0,G16/G25)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H34" s="2">
-        <f>IF(H25=0,0,H16/H25)</f>
+        <f t="shared" si="10"/>
         <v>-372.63</v>
       </c>
       <c r="I34" s="2">
-        <f>IF(I25=0,0,I16/I25)</f>
+        <f t="shared" si="10"/>
         <v>-3.165975</v>
       </c>
       <c r="J34" s="2">
-        <f>IF(J25=0,0,J16/J25)</f>
+        <f t="shared" si="10"/>
         <v>-208.42376666666667</v>
       </c>
     </row>
@@ -1956,71 +1956,71 @@
         <v>2</v>
       </c>
       <c r="C35" s="2">
-        <f>IF(C26=0,0,C17/C26)</f>
+        <f t="shared" si="10"/>
         <v>1125.57</v>
       </c>
       <c r="D35" s="2">
-        <f>IF(D26=0,0,D17/D26)</f>
-        <v>-211.1465</v>
+        <f t="shared" si="10"/>
+        <v>-210.43947368421053</v>
       </c>
       <c r="E35" s="2">
-        <f>IF(E26=0,0,E17/E26)</f>
-        <v>102.86</v>
+        <f t="shared" si="10"/>
+        <v>89.889166666666668</v>
       </c>
       <c r="F35" s="2">
-        <f>IF(F26=0,0,F17/F26)</f>
-        <v>57.249791666666653</v>
+        <f t="shared" si="10"/>
+        <v>56.622765957446809</v>
       </c>
       <c r="G35" s="2">
-        <f>IF(G26=0,0,G17/G26)</f>
-        <v>502.23599999999999</v>
+        <f t="shared" si="10"/>
+        <v>647.47666666666669</v>
       </c>
       <c r="H35" s="2">
-        <f>IF(H26=0,0,H17/H26)</f>
+        <f t="shared" si="10"/>
         <v>-169.36750000000001</v>
       </c>
       <c r="I35" s="2">
-        <f>IF(I26=0,0,I17/I26)</f>
+        <f t="shared" si="10"/>
         <v>63.072384615384621</v>
       </c>
       <c r="J35" s="2">
-        <f>IF(J26=0,0,J17/J26)</f>
-        <v>18.271794117647051</v>
+        <f t="shared" si="10"/>
+        <v>1.6403437499999995</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B36" s="3"/>
       <c r="C36" s="3">
         <f>C18/C27</f>
-        <v>620.65556818181824</v>
+        <v>640.79867469879514</v>
       </c>
       <c r="D36" s="3">
-        <f t="shared" ref="D36:J36" si="10">D18/D27</f>
-        <v>-291.91150943396224</v>
+        <f t="shared" ref="D36:J36" si="11">D18/D27</f>
+        <v>-295.80995215311003</v>
       </c>
       <c r="E36" s="3">
-        <f t="shared" si="10"/>
-        <v>157.32132420091327</v>
+        <f t="shared" si="11"/>
+        <v>150.66806763285024</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" si="10"/>
-        <v>52.38115606936416</v>
+        <f t="shared" si="11"/>
+        <v>45.190981963927854</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="10"/>
-        <v>542.88597560975597</v>
+        <f t="shared" si="11"/>
+        <v>597.26567164179096</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="10"/>
-        <v>-263.3343023255814</v>
+        <f t="shared" si="11"/>
+        <v>-246.94506250000001</v>
       </c>
       <c r="I36" s="3">
-        <f t="shared" si="10"/>
-        <v>38.696107619047616</v>
+        <f t="shared" si="11"/>
+        <v>54.076159374999996</v>
       </c>
       <c r="J36" s="3">
-        <f t="shared" si="10"/>
-        <v>9.1538754874651804</v>
+        <f t="shared" si="11"/>
+        <v>17.637465325077397</v>
       </c>
     </row>
   </sheetData>
@@ -2047,7 +2047,7 @@
   <dimension ref="B2:J36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2090,30 +2090,30 @@
       </c>
       <c r="C3" s="2">
         <f>F13</f>
-        <v>4893.4400000000014</v>
+        <v>2735.95</v>
       </c>
       <c r="D3" s="2">
         <f>J13</f>
-        <v>6285.0399999999991</v>
+        <v>5194.420000000001</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3:E8" si="0">D3+C3</f>
-        <v>11178.48</v>
+        <v>7930.3700000000008</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
       </c>
       <c r="H3" s="2">
         <f>F22</f>
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I3" s="2">
         <f>J22</f>
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ref="J3:J8" si="1">I3+H3</f>
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
@@ -2122,30 +2122,30 @@
       </c>
       <c r="C4" s="2">
         <f>F14</f>
-        <v>8588.7999999999956</v>
+        <v>8735.7999999999993</v>
       </c>
       <c r="D4" s="2">
         <f>J14</f>
-        <v>16291.459999999995</v>
+        <v>15285.559999999998</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>24880.259999999991</v>
+        <v>24021.359999999997</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="2">
         <f>F23</f>
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="I4" s="2">
         <f>J23</f>
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="1"/>
-        <v>562</v>
+        <v>538</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ref="C5:C7" si="2">F15</f>
-        <v>804.14000000000033</v>
+        <v>992.12999999999988</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" ref="D5:D7" si="3">J15</f>
@@ -2162,7 +2162,7 @@
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>-1129.8050000000003</v>
+        <v>-941.81500000000074</v>
       </c>
       <c r="G5" t="s">
         <v>0</v>
@@ -2186,7 +2186,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" si="2"/>
-        <v>913.93000000000006</v>
+        <v>659.05300000000011</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="3"/>
@@ -2194,7 +2194,7 @@
       </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>1146.5230000000001</v>
+        <v>891.64600000000019</v>
       </c>
       <c r="G6" t="s">
         <v>1</v>
@@ -2218,7 +2218,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" si="2"/>
-        <v>1805.46</v>
+        <v>1980.9599999999996</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="3"/>
@@ -2226,14 +2226,14 @@
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>-930.81999999999971</v>
+        <v>-755.32000000000016</v>
       </c>
       <c r="G7" t="s">
         <v>2</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="4"/>
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="5"/>
@@ -2241,35 +2241,35 @@
       </c>
       <c r="J7" s="2">
         <f t="shared" si="1"/>
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
       <c r="C8" s="3">
         <f>SUM(C3:C7)</f>
-        <v>17005.769999999997</v>
+        <v>15103.892999999998</v>
       </c>
       <c r="D8" s="3">
         <f>SUM(D3:D7)</f>
-        <v>18138.867999999995</v>
+        <v>16042.348000000002</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
-        <v>35144.637999999992</v>
+        <v>31146.241000000002</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3">
         <f>SUM(H4:H7)</f>
-        <v>480</v>
+        <v>469</v>
       </c>
       <c r="I8" s="3">
         <f>SUM(I4:I7)</f>
-        <v>472</v>
+        <v>457</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" si="1"/>
-        <v>952</v>
+        <v>926</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
@@ -2278,32 +2278,32 @@
       </c>
       <c r="C9" s="1">
         <f>C8/1000000*12/COUNT(C3:C7)</f>
-        <v>4.0813847999999993E-2</v>
+        <v>3.6249343199999992E-2</v>
       </c>
       <c r="D9" s="1">
         <f>D8/1000000*12/COUNT(D3:D7)</f>
-        <v>4.3533283199999988E-2</v>
+        <v>3.8501635200000009E-2</v>
       </c>
       <c r="E9" s="1">
         <f>E8/1000000*12/COUNT(E3:E7)</f>
-        <v>8.4347131199999981E-2</v>
+        <v>7.4750978400000001E-2</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4" t="s">
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2320,7 +2320,7 @@
       <c r="E12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="3" t="s">
         <v>10</v>
       </c>
@@ -2330,37 +2330,37 @@
       <c r="I12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="4"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="2">
-        <v>13672.9</v>
+        <v>12995.9</v>
       </c>
       <c r="D13" s="2">
-        <v>-16652.599999999999</v>
+        <v>-16984</v>
       </c>
       <c r="E13" s="2">
-        <v>7873.14</v>
+        <v>6724.05</v>
       </c>
       <c r="F13" s="2">
         <f>SUM(C13:E13)</f>
-        <v>4893.4400000000014</v>
+        <v>2735.95</v>
       </c>
       <c r="G13" s="2">
-        <v>18589.099999999999</v>
+        <v>17517.7</v>
       </c>
       <c r="H13" s="2">
         <v>-13841</v>
       </c>
       <c r="I13" s="2">
-        <v>1536.94</v>
+        <v>1517.72</v>
       </c>
       <c r="J13" s="2">
         <f>SUM(G13:I13)</f>
-        <v>6285.0399999999991</v>
+        <v>5194.420000000001</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
@@ -2368,30 +2368,30 @@
         <v>3</v>
       </c>
       <c r="C14" s="2">
-        <v>29216.6</v>
+        <v>29601.5</v>
       </c>
       <c r="D14" s="2">
-        <v>-32839.800000000003</v>
+        <v>-31895.200000000001</v>
       </c>
       <c r="E14" s="2">
-        <v>12212</v>
+        <v>11029.5</v>
       </c>
       <c r="F14" s="2">
         <f>SUM(C14:E14)</f>
-        <v>8588.7999999999956</v>
+        <v>8735.7999999999993</v>
       </c>
       <c r="G14" s="2">
-        <v>36755.199999999997</v>
+        <v>34330.6</v>
       </c>
       <c r="H14" s="2">
-        <v>-25721.200000000001</v>
+        <v>-24302.5</v>
       </c>
       <c r="I14" s="2">
         <v>5257.46</v>
       </c>
       <c r="J14" s="2">
         <f>SUM(G14:I14)</f>
-        <v>16291.459999999995</v>
+        <v>15285.559999999998</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
@@ -2399,17 +2399,17 @@
         <v>0</v>
       </c>
       <c r="C15" s="2">
-        <v>5938.21</v>
+        <v>6498.68</v>
       </c>
       <c r="D15" s="2">
-        <v>-6704.44</v>
+        <v>-6695.77</v>
       </c>
       <c r="E15" s="2">
-        <v>1570.37</v>
+        <v>1189.22</v>
       </c>
       <c r="F15" s="2">
         <f>SUM(C15:E15)</f>
-        <v>804.14000000000033</v>
+        <v>992.12999999999988</v>
       </c>
       <c r="G15" s="2">
         <v>2704.95</v>
@@ -2436,11 +2436,11 @@
         <v>-1996.34</v>
       </c>
       <c r="E16" s="2">
-        <v>1212.5999999999999</v>
+        <v>957.72299999999996</v>
       </c>
       <c r="F16" s="2">
         <f>SUM(C16:E16)</f>
-        <v>913.93000000000006</v>
+        <v>659.05300000000011</v>
       </c>
       <c r="G16" s="2">
         <v>3120.19</v>
@@ -2461,17 +2461,17 @@
         <v>2</v>
       </c>
       <c r="C17" s="2">
-        <v>9561.41</v>
+        <v>9424.25</v>
       </c>
       <c r="D17" s="2">
-        <v>-9262.83</v>
+        <v>-9084.85</v>
       </c>
       <c r="E17" s="2">
-        <v>1506.88</v>
+        <v>1641.56</v>
       </c>
       <c r="F17" s="2">
         <f>SUM(C17:E17)</f>
-        <v>1805.46</v>
+        <v>1980.9599999999996</v>
       </c>
       <c r="G17" s="2">
         <v>7741.72</v>
@@ -2491,52 +2491,52 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3">
         <f>SUM(C13:C17)</f>
-        <v>60086.789999999994</v>
+        <v>60218</v>
       </c>
       <c r="D18" s="3">
         <f t="shared" ref="D18:J18" si="6">SUM(D13:D17)</f>
-        <v>-67456.009999999995</v>
+        <v>-66656.160000000003</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" si="6"/>
-        <v>24374.989999999998</v>
+        <v>21542.053000000004</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="6"/>
-        <v>17005.769999999997</v>
+        <v>15103.892999999998</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="6"/>
-        <v>68911.159999999989</v>
+        <v>65415.16</v>
       </c>
       <c r="H18" s="3">
         <f t="shared" si="6"/>
-        <v>-59155.42</v>
+        <v>-57736.72</v>
       </c>
       <c r="I18" s="3">
         <f t="shared" si="6"/>
-        <v>8383.1279999999988</v>
+        <v>8363.9079999999994</v>
       </c>
       <c r="J18" s="3">
         <f t="shared" si="6"/>
-        <v>18138.867999999995</v>
+        <v>16042.348000000002</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4" t="s">
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2553,7 +2553,7 @@
       <c r="E21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="3" t="s">
         <v>10</v>
       </c>
@@ -2563,37 +2563,37 @@
       <c r="I21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J21" s="4"/>
+      <c r="J21" s="5"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C22" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="2">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E22" s="2">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F22" s="2">
         <f>SUM(C22:E22)</f>
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G22" s="2">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H22" s="2">
         <v>103</v>
       </c>
       <c r="I22" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J22" s="2">
         <f>SUM(G22:I22)</f>
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
@@ -2604,27 +2604,27 @@
         <v>51</v>
       </c>
       <c r="D23" s="2">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E23" s="2">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F23" s="2">
         <f>SUM(C23:E23)</f>
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="G23" s="2">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H23" s="2">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I23" s="2">
         <v>36</v>
       </c>
       <c r="J23" s="2">
         <f>SUM(G23:I23)</f>
-        <v>273</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
@@ -2632,13 +2632,13 @@
         <v>0</v>
       </c>
       <c r="C24" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D24" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E24" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F24" s="2">
         <f>SUM(C24:E24)</f>
@@ -2697,14 +2697,14 @@
         <v>11</v>
       </c>
       <c r="D26" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E26" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" s="2">
         <f>SUM(C26:E26)</f>
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G26" s="2">
         <v>17</v>
@@ -2728,48 +2728,48 @@
       </c>
       <c r="D27" s="3">
         <f t="shared" ref="D27:J27" si="7">SUM(D22:D26)</f>
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" si="7"/>
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="7"/>
-        <v>650</v>
+        <v>636</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="7"/>
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="H27" s="3">
         <f t="shared" si="7"/>
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I27" s="3">
         <f t="shared" si="7"/>
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J27" s="3">
         <f t="shared" si="7"/>
-        <v>628</v>
+        <v>609</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4" t="s">
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4" t="s">
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2786,7 +2786,7 @@
       <c r="E30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="4"/>
+      <c r="F30" s="5"/>
       <c r="G30" s="3" t="s">
         <v>10</v>
       </c>
@@ -2796,43 +2796,43 @@
       <c r="I30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J30" s="4"/>
+      <c r="J30" s="5"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="2">
-        <f>IF(C22=0,0,C13/C22)</f>
-        <v>621.49545454545455</v>
+        <f t="shared" ref="C31:J35" si="8">IF(C22=0,0,C13/C22)</f>
+        <v>618.85238095238094</v>
       </c>
       <c r="D31" s="2">
-        <f>IF(D22=0,0,D13/D22)</f>
-        <v>-144.80521739130432</v>
+        <f t="shared" si="8"/>
+        <v>-145.16239316239316</v>
       </c>
       <c r="E31" s="2">
-        <f>IF(E22=0,0,E13/E22)</f>
-        <v>238.58</v>
+        <f t="shared" si="8"/>
+        <v>231.86379310344827</v>
       </c>
       <c r="F31" s="2">
-        <f>IF(F22=0,0,F13/F22)</f>
-        <v>28.784941176470596</v>
+        <f t="shared" si="8"/>
+        <v>16.382934131736526</v>
       </c>
       <c r="G31" s="2">
-        <f>IF(G22=0,0,G13/G22)</f>
-        <v>489.18684210526311</v>
+        <f t="shared" si="8"/>
+        <v>500.5057142857143</v>
       </c>
       <c r="H31" s="2">
-        <f>IF(H22=0,0,H13/H22)</f>
+        <f t="shared" si="8"/>
         <v>-134.37864077669903</v>
       </c>
       <c r="I31" s="2">
-        <f>IF(I22=0,0,I13/I22)</f>
-        <v>102.46266666666666</v>
+        <f t="shared" si="8"/>
+        <v>108.40857142857143</v>
       </c>
       <c r="J31" s="2">
-        <f>IF(J22=0,0,J13/J22)</f>
-        <v>40.288717948717945</v>
+        <f t="shared" si="8"/>
+        <v>34.173815789473693</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
@@ -2840,36 +2840,36 @@
         <v>3</v>
       </c>
       <c r="C32" s="2">
-        <f>IF(C23=0,0,C14/C23)</f>
-        <v>572.87450980392157</v>
+        <f t="shared" si="8"/>
+        <v>580.42156862745094</v>
       </c>
       <c r="D32" s="2">
-        <f>IF(D23=0,0,D14/D23)</f>
-        <v>-173.75555555555556</v>
+        <f t="shared" si="8"/>
+        <v>-173.34347826086957</v>
       </c>
       <c r="E32" s="2">
-        <f>IF(E23=0,0,E14/E23)</f>
-        <v>249.22448979591837</v>
+        <f t="shared" si="8"/>
+        <v>245.1</v>
       </c>
       <c r="F32" s="2">
-        <f>IF(F23=0,0,F14/F23)</f>
-        <v>29.719031141868498</v>
+        <f t="shared" si="8"/>
+        <v>31.199285714285711</v>
       </c>
       <c r="G32" s="2">
-        <f>IF(G23=0,0,G14/G23)</f>
-        <v>490.0693333333333</v>
+        <f t="shared" si="8"/>
+        <v>536.41562499999998</v>
       </c>
       <c r="H32" s="2">
-        <f>IF(H23=0,0,H14/H23)</f>
-        <v>-158.77283950617286</v>
+        <f t="shared" si="8"/>
+        <v>-153.8132911392405</v>
       </c>
       <c r="I32" s="2">
-        <f>IF(I23=0,0,I14/I23)</f>
+        <f t="shared" si="8"/>
         <v>146.04055555555556</v>
       </c>
       <c r="J32" s="2">
-        <f>IF(J23=0,0,J14/J23)</f>
-        <v>59.675677655677639</v>
+        <f t="shared" si="8"/>
+        <v>59.246356589147275</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
@@ -2877,35 +2877,35 @@
         <v>0</v>
       </c>
       <c r="C33" s="2">
-        <f>IF(C24=0,0,C15/C24)</f>
-        <v>848.31571428571431</v>
+        <f t="shared" si="8"/>
+        <v>812.33500000000004</v>
       </c>
       <c r="D33" s="2">
-        <f>IF(D24=0,0,D15/D24)</f>
-        <v>-124.15629629629629</v>
+        <f t="shared" si="8"/>
+        <v>-121.74127272727273</v>
       </c>
       <c r="E33" s="2">
-        <f>IF(E24=0,0,E15/E24)</f>
-        <v>224.33857142857141</v>
+        <f t="shared" si="8"/>
+        <v>237.84399999999999</v>
       </c>
       <c r="F33" s="2">
-        <f>IF(F24=0,0,F15/F24)</f>
-        <v>11.825588235294122</v>
+        <f t="shared" si="8"/>
+        <v>14.590147058823527</v>
       </c>
       <c r="G33" s="2">
-        <f>IF(G24=0,0,G15/G24)</f>
+        <f t="shared" si="8"/>
         <v>386.42142857142852</v>
       </c>
       <c r="H33" s="2">
-        <f>IF(H24=0,0,H15/H24)</f>
+        <f t="shared" si="8"/>
         <v>-127.40659090909092</v>
       </c>
       <c r="I33" s="2">
-        <f>IF(I24=0,0,I15/I24)</f>
+        <f t="shared" si="8"/>
         <v>161.16583333333332</v>
       </c>
       <c r="J33" s="2">
-        <f>IF(J24=0,0,J15/J24)</f>
+        <f t="shared" si="8"/>
         <v>-33.92885964912282</v>
       </c>
     </row>
@@ -2914,35 +2914,35 @@
         <v>1</v>
       </c>
       <c r="C34" s="2">
-        <f>IF(C25=0,0,C16/C25)</f>
+        <f t="shared" si="8"/>
         <v>565.89</v>
       </c>
       <c r="D34" s="2">
-        <f>IF(D25=0,0,D16/D25)</f>
+        <f t="shared" si="8"/>
         <v>-117.43176470588234</v>
       </c>
       <c r="E34" s="2">
-        <f>IF(E25=0,0,E16/E25)</f>
-        <v>242.51999999999998</v>
+        <f t="shared" si="8"/>
+        <v>191.5446</v>
       </c>
       <c r="F34" s="2">
-        <f>IF(F25=0,0,F16/F25)</f>
-        <v>36.557200000000002</v>
+        <f t="shared" si="8"/>
+        <v>26.362120000000004</v>
       </c>
       <c r="G34" s="2">
-        <f>IF(G25=0,0,G16/G25)</f>
+        <f t="shared" si="8"/>
         <v>390.02375000000001</v>
       </c>
       <c r="H34" s="2">
-        <f>IF(H25=0,0,H16/H25)</f>
+        <f t="shared" si="8"/>
         <v>-134.97423076923076</v>
       </c>
       <c r="I34" s="2">
-        <f>IF(I25=0,0,I16/I25)</f>
+        <f t="shared" si="8"/>
         <v>155.43324999999999</v>
       </c>
       <c r="J34" s="2">
-        <f>IF(J25=0,0,J16/J25)</f>
+        <f t="shared" si="8"/>
         <v>6.1208684210526334</v>
       </c>
     </row>
@@ -2951,35 +2951,35 @@
         <v>2</v>
       </c>
       <c r="C35" s="2">
-        <f>IF(C26=0,0,C17/C26)</f>
-        <v>869.21909090909094</v>
+        <f t="shared" si="8"/>
+        <v>856.75</v>
       </c>
       <c r="D35" s="2">
-        <f>IF(D26=0,0,D17/D26)</f>
-        <v>-117.25101265822785</v>
+        <f t="shared" si="8"/>
+        <v>-116.4724358974359</v>
       </c>
       <c r="E35" s="2">
-        <f>IF(E26=0,0,E17/E26)</f>
-        <v>188.36</v>
+        <f t="shared" si="8"/>
+        <v>234.50857142857143</v>
       </c>
       <c r="F35" s="2">
-        <f>IF(F26=0,0,F17/F26)</f>
-        <v>18.423061224489796</v>
+        <f t="shared" si="8"/>
+        <v>20.634999999999994</v>
       </c>
       <c r="G35" s="2">
-        <f>IF(G26=0,0,G17/G26)</f>
+        <f t="shared" si="8"/>
         <v>455.3952941176471</v>
       </c>
       <c r="H35" s="2">
-        <f>IF(H26=0,0,H17/H26)</f>
+        <f t="shared" si="8"/>
         <v>-120.43678160919541</v>
       </c>
       <c r="I35" s="2">
-        <f>IF(I26=0,0,I17/I26)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J35" s="2">
-        <f>IF(J26=0,0,J17/J26)</f>
+        <f t="shared" si="8"/>
         <v>-26.310384615384613</v>
       </c>
     </row>
@@ -2987,35 +2987,35 @@
       <c r="B36" s="3"/>
       <c r="C36" s="3">
         <f>C18/C27</f>
-        <v>639.22117021276586</v>
+        <v>640.61702127659578</v>
       </c>
       <c r="D36" s="3">
-        <f t="shared" ref="D36:J36" si="8">D18/D27</f>
-        <v>-148.58151982378854</v>
+        <f t="shared" ref="D36:J36" si="9">D18/D27</f>
+        <v>-147.79636363636365</v>
       </c>
       <c r="E36" s="3">
-        <f t="shared" si="8"/>
-        <v>238.9704901960784</v>
+        <f t="shared" si="9"/>
+        <v>236.72585714285719</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" si="8"/>
-        <v>26.162723076923072</v>
+        <f t="shared" si="9"/>
+        <v>23.748259433962261</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="8"/>
-        <v>475.24937931034475</v>
+        <f t="shared" si="9"/>
+        <v>499.35236641221377</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="8"/>
-        <v>-140.17872037914691</v>
+        <f t="shared" si="9"/>
+        <v>-138.12612440191387</v>
       </c>
       <c r="I36" s="3">
-        <f t="shared" si="8"/>
-        <v>137.42832786885245</v>
+        <f t="shared" si="9"/>
+        <v>139.39846666666665</v>
       </c>
       <c r="J36" s="3">
-        <f t="shared" si="8"/>
-        <v>28.883547770700631</v>
+        <f t="shared" si="9"/>
+        <v>26.342114942528738</v>
       </c>
     </row>
   </sheetData>

</xml_diff>